<commit_message>
login, signuup logic, request data, accountSetting data
</commit_message>
<xml_diff>
--- a/backend/src/assets/test/football.xlsx
+++ b/backend/src/assets/test/football.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project_int3509\backend\src\controllers\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0FFEB7-4209-40F4-A26E-69D4ACE40DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D8C457-C6D5-46B1-801E-B608CA7B7AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{F2802D8D-390D-4525-909C-B8B5158C3A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="75">
   <si>
     <t>Bùi Tuấn Anh</t>
   </si>
@@ -260,7 +260,7 @@
     <t>trường</t>
   </si>
   <si>
-    <t>bóng rổ</t>
+    <t>bóng chuyền da</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -770,7 +770,7 @@
         <v>70</v>
       </c>
       <c r="E2" s="9">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -787,7 +787,7 @@
         <v>70</v>
       </c>
       <c r="E3" s="9">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -804,7 +804,7 @@
         <v>70</v>
       </c>
       <c r="E4" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -838,7 +838,7 @@
         <v>70</v>
       </c>
       <c r="E6" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -855,7 +855,7 @@
         <v>70</v>
       </c>
       <c r="E7" s="9">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -872,7 +872,7 @@
         <v>70</v>
       </c>
       <c r="E8" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -889,7 +889,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -906,7 +906,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -923,7 +923,7 @@
         <v>70</v>
       </c>
       <c r="E11" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -940,7 +940,7 @@
         <v>70</v>
       </c>
       <c r="E12" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -957,7 +957,7 @@
         <v>70</v>
       </c>
       <c r="E13" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -974,7 +974,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -991,7 +991,7 @@
         <v>70</v>
       </c>
       <c r="E15" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1008,7 +1008,7 @@
         <v>70</v>
       </c>
       <c r="E16" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1025,7 +1025,7 @@
         <v>70</v>
       </c>
       <c r="E17" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1042,7 +1042,7 @@
         <v>70</v>
       </c>
       <c r="E18" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1059,7 +1059,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1076,7 +1076,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1093,7 +1093,7 @@
         <v>70</v>
       </c>
       <c r="E21" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1110,7 +1110,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1127,7 +1127,7 @@
         <v>70</v>
       </c>
       <c r="E23" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1144,7 +1144,7 @@
         <v>70</v>
       </c>
       <c r="E24" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1161,7 +1161,7 @@
         <v>70</v>
       </c>
       <c r="E25" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1178,7 +1178,7 @@
         <v>70</v>
       </c>
       <c r="E26" s="9">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1195,7 +1195,7 @@
         <v>70</v>
       </c>
       <c r="E27" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1212,7 +1212,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1229,7 +1229,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1246,7 +1246,7 @@
         <v>70</v>
       </c>
       <c r="E30" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1263,7 +1263,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1280,7 +1280,7 @@
         <v>70</v>
       </c>
       <c r="E32" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31" x14ac:dyDescent="0.35">
@@ -1297,7 +1297,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1314,7 +1314,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1331,7 +1331,7 @@
         <v>70</v>
       </c>
       <c r="E35" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1348,7 +1348,7 @@
         <v>70</v>
       </c>
       <c r="E36" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1365,7 +1365,7 @@
         <v>70</v>
       </c>
       <c r="E37" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
       <c r="E38" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1399,7 +1399,7 @@
         <v>70</v>
       </c>
       <c r="E39" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1416,7 +1416,7 @@
         <v>70</v>
       </c>
       <c r="E40" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1433,7 +1433,7 @@
         <v>70</v>
       </c>
       <c r="E41" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1450,7 +1450,7 @@
         <v>70</v>
       </c>
       <c r="E42" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1467,7 +1467,7 @@
         <v>70</v>
       </c>
       <c r="E43" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1484,7 +1484,7 @@
         <v>70</v>
       </c>
       <c r="E44" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1501,7 +1501,7 @@
         <v>70</v>
       </c>
       <c r="E45" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1518,7 +1518,7 @@
         <v>70</v>
       </c>
       <c r="E46" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1535,7 +1535,7 @@
         <v>70</v>
       </c>
       <c r="E47" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1552,7 +1552,7 @@
         <v>70</v>
       </c>
       <c r="E48" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>70</v>
       </c>
       <c r="E49" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1586,7 +1586,7 @@
         <v>70</v>
       </c>
       <c r="E50" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1603,7 +1603,7 @@
         <v>70</v>
       </c>
       <c r="E51" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1620,7 +1620,7 @@
         <v>70</v>
       </c>
       <c r="E52" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1637,7 +1637,7 @@
         <v>70</v>
       </c>
       <c r="E53" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1654,7 +1654,7 @@
         <v>70</v>
       </c>
       <c r="E54" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1671,7 +1671,7 @@
         <v>70</v>
       </c>
       <c r="E55" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1688,7 +1688,7 @@
         <v>70</v>
       </c>
       <c r="E56" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1705,7 +1705,7 @@
         <v>70</v>
       </c>
       <c r="E57" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1722,7 +1722,7 @@
         <v>70</v>
       </c>
       <c r="E58" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1739,7 +1739,7 @@
         <v>70</v>
       </c>
       <c r="E59" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1756,7 +1756,7 @@
         <v>70</v>
       </c>
       <c r="E60" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1773,7 +1773,7 @@
         <v>70</v>
       </c>
       <c r="E61" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1790,7 +1790,7 @@
         <v>70</v>
       </c>
       <c r="E62" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1807,7 +1807,7 @@
         <v>70</v>
       </c>
       <c r="E63" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1824,7 +1824,7 @@
         <v>70</v>
       </c>
       <c r="E64" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1841,7 +1841,7 @@
         <v>70</v>
       </c>
       <c r="E65" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1858,7 +1858,7 @@
         <v>70</v>
       </c>
       <c r="E66" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1875,7 +1875,7 @@
         <v>70</v>
       </c>
       <c r="E67" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1892,7 +1892,7 @@
         <v>70</v>
       </c>
       <c r="E68" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1909,7 +1909,7 @@
         <v>70</v>
       </c>
       <c r="E69" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -1926,7 +1926,7 @@
         <v>70</v>
       </c>
       <c r="E70" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>